<commit_message>
update IEA scenarios with WEO2023
</commit_message>
<xml_diff>
--- a/Concordances/IEA_sectors_pathways_concordance .xlsx
+++ b/Concordances/IEA_sectors_pathways_concordance .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cstbgroup-my.sharepoint.com/personal/marin_pellan_cstb_fr/Documents/Thèse stratégie carbone/Articles/Journal_papers/Carbon_budgets_Building_Environment/French_WLC_budgets/Concordances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_AD4D9D64A577C15A4A5418E8901D7D545ADEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B897874-1BA1-4180-81A8-48240A3F7A93}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="11_AD4D9D64A577C15A4A5418E8901D7D545ADEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{569E790A-B7F7-4800-8C7D-C7595CEFA9D5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +216,12 @@
       <color rgb="FFC00000"/>
       <name val="Times"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +243,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEAF0F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -343,16 +353,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -361,18 +365,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,13 +683,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -685,10 +714,12 @@
     <col min="18" max="18" width="6.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.109375" style="5"/>
+    <col min="21" max="21" width="9.109375" style="5"/>
+    <col min="22" max="16384" width="9.109375" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
@@ -747,7 +778,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -808,8 +839,12 @@
       <c r="T2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W2" s="5">
+        <f>SUM(B2:T2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -870,70 +905,80 @@
       <c r="T3" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="W3" s="5">
+        <f t="shared" ref="W3:W34" si="0">SUM(B3:T3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5">
-        <v>0</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="O4" s="22">
+      <c r="B4" s="19">
+        <v>0</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20">
+        <v>0</v>
+      </c>
+      <c r="H4" s="19">
+        <v>0</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0</v>
+      </c>
+      <c r="J4" s="19">
+        <v>0</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0</v>
+      </c>
+      <c r="L4" s="19">
+        <v>0</v>
+      </c>
+      <c r="M4" s="19">
+        <v>0</v>
+      </c>
+      <c r="N4" s="19">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21">
         <v>1</v>
       </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>0</v>
-      </c>
-      <c r="R4" s="5">
-        <v>0</v>
-      </c>
-      <c r="S4" s="5">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P4" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>0</v>
+      </c>
+      <c r="R4" s="19">
+        <v>0</v>
+      </c>
+      <c r="S4" s="19">
+        <v>0</v>
+      </c>
+      <c r="T4" s="19">
+        <v>0</v>
+      </c>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -955,7 +1000,7 @@
       <c r="G5" s="3">
         <v>0</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="17">
         <v>1</v>
       </c>
       <c r="I5" s="5">
@@ -994,8 +1039,12 @@
       <c r="T5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W5" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -1056,8 +1105,12 @@
       <c r="T6" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1118,8 +1171,12 @@
       <c r="T7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1180,8 +1237,12 @@
       <c r="T8" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
@@ -1242,8 +1303,12 @@
       <c r="T9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="5">
         <v>0</v>
@@ -1302,71 +1367,81 @@
       <c r="T10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="W10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="22">
+      <c r="B11" s="19">
+        <v>0</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0</v>
+      </c>
+      <c r="F11" s="21">
         <v>1</v>
       </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
-      <c r="M11" s="5">
-        <v>0</v>
-      </c>
-      <c r="N11" s="5">
-        <v>0</v>
-      </c>
-      <c r="O11" s="5">
-        <v>0</v>
-      </c>
-      <c r="P11" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>0</v>
-      </c>
-      <c r="R11" s="5">
-        <v>0</v>
-      </c>
-      <c r="S11" s="22">
+      <c r="G11" s="20">
+        <v>0</v>
+      </c>
+      <c r="H11" s="19">
+        <v>0</v>
+      </c>
+      <c r="I11" s="19">
+        <v>0</v>
+      </c>
+      <c r="J11" s="19">
+        <v>0</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+      <c r="L11" s="19">
+        <v>0</v>
+      </c>
+      <c r="M11" s="19">
+        <v>0</v>
+      </c>
+      <c r="N11" s="19">
+        <v>0</v>
+      </c>
+      <c r="O11" s="19">
+        <v>0</v>
+      </c>
+      <c r="P11" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="19">
+        <v>0</v>
+      </c>
+      <c r="R11" s="19">
+        <v>0</v>
+      </c>
+      <c r="S11" s="21">
         <v>1</v>
       </c>
-      <c r="T11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="T11" s="19">
+        <v>0</v>
+      </c>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="5">
@@ -1426,9 +1501,13 @@
       <c r="T12" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="W12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="5">
@@ -1488,9 +1567,13 @@
       <c r="T13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="W13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="5">
@@ -1550,9 +1633,13 @@
       <c r="T14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="W14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="5">
@@ -1612,9 +1699,13 @@
       <c r="T15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="W15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="5">
@@ -1674,73 +1765,83 @@
       <c r="T16" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="W16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="27">
         <v>1</v>
       </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-      <c r="M17" s="5">
-        <v>0</v>
-      </c>
-      <c r="N17" s="5">
-        <v>0</v>
-      </c>
-      <c r="O17" s="5">
-        <v>0</v>
-      </c>
-      <c r="P17" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="5">
-        <v>0</v>
-      </c>
-      <c r="R17" s="5">
-        <v>0</v>
-      </c>
-      <c r="S17" s="5">
-        <v>0</v>
-      </c>
-      <c r="T17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="C17" s="19">
+        <v>0</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0</v>
+      </c>
+      <c r="E17" s="19">
         <v>1</v>
       </c>
+      <c r="F17" s="19">
+        <v>0</v>
+      </c>
+      <c r="G17" s="20">
+        <v>0</v>
+      </c>
+      <c r="H17" s="19">
+        <v>0</v>
+      </c>
+      <c r="I17" s="19">
+        <v>0</v>
+      </c>
+      <c r="J17" s="19">
+        <v>0</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="19">
+        <v>0</v>
+      </c>
+      <c r="M17" s="19">
+        <v>0</v>
+      </c>
+      <c r="N17" s="19">
+        <v>0</v>
+      </c>
+      <c r="O17" s="19">
+        <v>0</v>
+      </c>
+      <c r="P17" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="19">
+        <v>0</v>
+      </c>
+      <c r="R17" s="19">
+        <v>0</v>
+      </c>
+      <c r="S17" s="19">
+        <v>0</v>
+      </c>
+      <c r="T17" s="19">
+        <v>0</v>
+      </c>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>1</v>
+      </c>
       <c r="B18" s="5">
         <v>0</v>
       </c>
@@ -1798,9 +1899,13 @@
       <c r="T18" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="W18" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="5">
@@ -1860,9 +1965,13 @@
       <c r="T19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="W19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="5">
@@ -1880,7 +1989,7 @@
       <c r="F20" s="5">
         <v>0</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="14">
         <v>0</v>
       </c>
       <c r="H20" s="5">
@@ -1922,9 +2031,13 @@
       <c r="T20" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="W20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="5">
@@ -1942,7 +2055,7 @@
       <c r="F21" s="5">
         <v>0</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="15">
         <v>0</v>
       </c>
       <c r="H21" s="5">
@@ -1984,132 +2097,146 @@
       <c r="T21" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+      <c r="W21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="5">
-        <v>0</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0</v>
-      </c>
-      <c r="D22" s="22">
+      <c r="B22" s="19">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19">
+        <v>0</v>
+      </c>
+      <c r="D22" s="21">
         <v>1</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21"/>
+      <c r="F22" s="19">
+        <v>0</v>
+      </c>
+      <c r="G22" s="23">
+        <v>0</v>
+      </c>
+      <c r="H22" s="19">
+        <v>0</v>
+      </c>
+      <c r="I22" s="19">
+        <v>0</v>
+      </c>
+      <c r="J22" s="21">
         <v>1</v>
       </c>
-      <c r="F22" s="5">
-        <v>0</v>
-      </c>
-      <c r="G22" s="17">
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
-        <v>0</v>
-      </c>
-      <c r="J22" s="22">
+      <c r="K22" s="21">
         <v>1</v>
       </c>
-      <c r="K22" s="22">
+      <c r="L22" s="21">
         <v>1</v>
       </c>
-      <c r="L22" s="22">
+      <c r="M22" s="21">
         <v>1</v>
       </c>
-      <c r="M22" s="22">
+      <c r="N22" s="21">
         <v>1</v>
       </c>
-      <c r="N22" s="22">
+      <c r="O22" s="19">
+        <v>0</v>
+      </c>
+      <c r="P22" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="19">
+        <v>0</v>
+      </c>
+      <c r="R22" s="21">
         <v>1</v>
       </c>
-      <c r="O22" s="5">
-        <v>0</v>
-      </c>
-      <c r="P22" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="5">
-        <v>0</v>
-      </c>
-      <c r="R22" s="22">
+      <c r="S22" s="19">
+        <v>0</v>
+      </c>
+      <c r="T22" s="21">
         <v>1</v>
       </c>
-      <c r="S22" s="5">
-        <v>0</v>
-      </c>
-      <c r="T22" s="22">
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0</v>
+      </c>
+      <c r="C23" s="19">
+        <v>0</v>
+      </c>
+      <c r="D23" s="19">
+        <v>0</v>
+      </c>
+      <c r="E23" s="19">
+        <v>0</v>
+      </c>
+      <c r="F23" s="19">
+        <v>0</v>
+      </c>
+      <c r="G23" s="23">
+        <v>0</v>
+      </c>
+      <c r="H23" s="19">
+        <v>0</v>
+      </c>
+      <c r="I23" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="5">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0</v>
-      </c>
-      <c r="G23" s="17">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-      <c r="I23" s="22">
+      <c r="J23" s="19">
+        <v>0</v>
+      </c>
+      <c r="K23" s="19">
+        <v>0</v>
+      </c>
+      <c r="L23" s="19">
+        <v>0</v>
+      </c>
+      <c r="M23" s="19">
+        <v>0</v>
+      </c>
+      <c r="N23" s="19">
+        <v>0</v>
+      </c>
+      <c r="O23" s="19">
+        <v>0</v>
+      </c>
+      <c r="P23" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="19">
+        <v>0</v>
+      </c>
+      <c r="R23" s="19">
+        <v>0</v>
+      </c>
+      <c r="S23" s="19">
+        <v>0</v>
+      </c>
+      <c r="T23" s="19">
+        <v>0</v>
+      </c>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="19">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J23" s="5">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5">
-        <v>0</v>
-      </c>
-      <c r="L23" s="5">
-        <v>0</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0</v>
-      </c>
-      <c r="N23" s="5">
-        <v>0</v>
-      </c>
-      <c r="O23" s="5">
-        <v>0</v>
-      </c>
-      <c r="P23" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="5">
-        <v>0</v>
-      </c>
-      <c r="R23" s="5">
-        <v>0</v>
-      </c>
-      <c r="S23" s="5">
-        <v>0</v>
-      </c>
-      <c r="T23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>13</v>
       </c>
@@ -2128,7 +2255,7 @@
       <c r="F24" s="5">
         <v>0</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="15">
         <v>0</v>
       </c>
       <c r="H24" s="5">
@@ -2170,195 +2297,214 @@
       <c r="T24" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="W24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="5">
-        <v>0</v>
-      </c>
-      <c r="C25" s="22">
+      <c r="B25" s="19">
+        <v>0</v>
+      </c>
+      <c r="C25" s="21">
         <v>1</v>
       </c>
-      <c r="D25" s="5">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
-        <v>0</v>
-      </c>
-      <c r="G25" s="17">
-        <v>0</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5">
-        <v>0</v>
-      </c>
-      <c r="J25" s="5">
-        <v>0</v>
-      </c>
-      <c r="K25" s="5">
-        <v>0</v>
-      </c>
-      <c r="L25" s="5">
-        <v>0</v>
-      </c>
-      <c r="M25" s="5">
-        <v>0</v>
-      </c>
-      <c r="N25" s="5">
-        <v>0</v>
-      </c>
-      <c r="O25" s="5">
-        <v>0</v>
-      </c>
-      <c r="P25" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="5">
-        <v>0</v>
-      </c>
-      <c r="R25" s="5">
-        <v>0</v>
-      </c>
-      <c r="S25" s="5">
-        <v>0</v>
-      </c>
-      <c r="T25" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="D25" s="19">
+        <v>0</v>
+      </c>
+      <c r="E25" s="19">
+        <v>0</v>
+      </c>
+      <c r="F25" s="19">
+        <v>0</v>
+      </c>
+      <c r="G25" s="23">
+        <v>0</v>
+      </c>
+      <c r="H25" s="19">
+        <v>0</v>
+      </c>
+      <c r="I25" s="19">
+        <v>0</v>
+      </c>
+      <c r="J25" s="19">
+        <v>0</v>
+      </c>
+      <c r="K25" s="19">
+        <v>0</v>
+      </c>
+      <c r="L25" s="19">
+        <v>0</v>
+      </c>
+      <c r="M25" s="19">
+        <v>0</v>
+      </c>
+      <c r="N25" s="19">
+        <v>0</v>
+      </c>
+      <c r="O25" s="19">
+        <v>0</v>
+      </c>
+      <c r="P25" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="19">
+        <v>0</v>
+      </c>
+      <c r="R25" s="19">
+        <v>0</v>
+      </c>
+      <c r="S25" s="19">
+        <v>0</v>
+      </c>
+      <c r="T25" s="19">
+        <v>0</v>
+      </c>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="5">
-        <v>0</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5">
-        <v>0</v>
-      </c>
-      <c r="G26" s="17">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5">
-        <v>0</v>
-      </c>
-      <c r="J26" s="5">
-        <v>0</v>
-      </c>
-      <c r="K26" s="5">
-        <v>0</v>
-      </c>
-      <c r="L26" s="5">
-        <v>0</v>
-      </c>
-      <c r="M26" s="5">
-        <v>0</v>
-      </c>
-      <c r="N26" s="5">
-        <v>0</v>
-      </c>
-      <c r="O26" s="5">
-        <v>0</v>
-      </c>
-      <c r="P26" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="22">
+      <c r="B26" s="28">
+        <v>0</v>
+      </c>
+      <c r="C26" s="28">
+        <v>0</v>
+      </c>
+      <c r="D26" s="28">
+        <v>0</v>
+      </c>
+      <c r="E26" s="28">
+        <v>0</v>
+      </c>
+      <c r="F26" s="28">
+        <v>0</v>
+      </c>
+      <c r="G26" s="30">
+        <v>0</v>
+      </c>
+      <c r="H26" s="28">
+        <v>0</v>
+      </c>
+      <c r="I26" s="28">
+        <v>0</v>
+      </c>
+      <c r="J26" s="28">
+        <v>0</v>
+      </c>
+      <c r="K26" s="28">
+        <v>0</v>
+      </c>
+      <c r="L26" s="28">
+        <v>0</v>
+      </c>
+      <c r="M26" s="28">
+        <v>0</v>
+      </c>
+      <c r="N26" s="28">
+        <v>0</v>
+      </c>
+      <c r="O26" s="28">
+        <v>0</v>
+      </c>
+      <c r="P26" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="31">
+        <v>0</v>
+      </c>
+      <c r="R26" s="28">
+        <v>0</v>
+      </c>
+      <c r="S26" s="28">
+        <v>0</v>
+      </c>
+      <c r="T26" s="28">
+        <v>0</v>
+      </c>
+      <c r="U26" s="28"/>
+      <c r="W26" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="19">
+        <v>0</v>
+      </c>
+      <c r="C27" s="19">
+        <v>0</v>
+      </c>
+      <c r="D27" s="19">
+        <v>0</v>
+      </c>
+      <c r="E27" s="19">
+        <v>0</v>
+      </c>
+      <c r="F27" s="19">
+        <v>0</v>
+      </c>
+      <c r="G27" s="19">
+        <v>0</v>
+      </c>
+      <c r="H27" s="19">
+        <v>0</v>
+      </c>
+      <c r="I27" s="19">
+        <v>0</v>
+      </c>
+      <c r="J27" s="19">
+        <v>0</v>
+      </c>
+      <c r="K27" s="19">
+        <v>0</v>
+      </c>
+      <c r="L27" s="19">
+        <v>0</v>
+      </c>
+      <c r="M27" s="19">
+        <v>0</v>
+      </c>
+      <c r="N27" s="19">
+        <v>0</v>
+      </c>
+      <c r="O27" s="19">
+        <v>0</v>
+      </c>
+      <c r="P27" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="21">
         <v>1</v>
       </c>
-      <c r="R26" s="5">
-        <v>0</v>
-      </c>
-      <c r="S26" s="5">
-        <v>0</v>
-      </c>
-      <c r="T26" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="5">
-        <v>0</v>
-      </c>
-      <c r="C27" s="5">
-        <v>0</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0</v>
-      </c>
-      <c r="G27" s="5">
-        <v>0</v>
-      </c>
-      <c r="H27" s="5">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
-        <v>0</v>
-      </c>
-      <c r="K27" s="5">
-        <v>0</v>
-      </c>
-      <c r="L27" s="5">
-        <v>0</v>
-      </c>
-      <c r="M27" s="5">
-        <v>0</v>
-      </c>
-      <c r="N27" s="5">
-        <v>0</v>
-      </c>
-      <c r="O27" s="5">
-        <v>0</v>
-      </c>
-      <c r="P27" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="5">
-        <v>0</v>
-      </c>
-      <c r="R27" s="5">
-        <v>0</v>
-      </c>
-      <c r="S27" s="5">
-        <v>0</v>
-      </c>
-      <c r="T27" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="R27" s="19">
+        <v>0</v>
+      </c>
+      <c r="S27" s="19">
+        <v>0</v>
+      </c>
+      <c r="T27" s="19">
+        <v>0</v>
+      </c>
+      <c r="W27" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="5">
@@ -2376,7 +2522,7 @@
       <c r="F28" s="5">
         <v>0</v>
       </c>
-      <c r="G28" s="17">
+      <c r="G28" s="15">
         <v>0</v>
       </c>
       <c r="H28" s="5">
@@ -2418,9 +2564,13 @@
       <c r="T28" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="W28" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="5">
@@ -2480,8 +2630,12 @@
       <c r="T29" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W29" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>19</v>
       </c>
@@ -2542,8 +2696,12 @@
       <c r="T30" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W30" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>20</v>
       </c>
@@ -2604,9 +2762,13 @@
       <c r="T31" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="W31" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="5">
@@ -2666,8 +2828,12 @@
       <c r="T32" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W32" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>22</v>
       </c>
@@ -2728,67 +2894,77 @@
       <c r="T33" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+      <c r="W33" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="5">
-        <v>0</v>
-      </c>
-      <c r="C34" s="5">
-        <v>0</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-      <c r="E34" s="5">
-        <v>0</v>
-      </c>
-      <c r="F34" s="5">
-        <v>0</v>
-      </c>
-      <c r="G34" s="22">
+      <c r="B34" s="19">
+        <v>0</v>
+      </c>
+      <c r="C34" s="19">
+        <v>0</v>
+      </c>
+      <c r="D34" s="19">
+        <v>0</v>
+      </c>
+      <c r="E34" s="19">
+        <v>0</v>
+      </c>
+      <c r="F34" s="19">
+        <v>0</v>
+      </c>
+      <c r="G34" s="21">
         <v>1</v>
       </c>
-      <c r="H34" s="5">
-        <v>0</v>
-      </c>
-      <c r="I34" s="5">
-        <v>0</v>
-      </c>
-      <c r="J34" s="5">
-        <v>0</v>
-      </c>
-      <c r="K34" s="5">
-        <v>0</v>
-      </c>
-      <c r="L34" s="5">
-        <v>0</v>
-      </c>
-      <c r="M34" s="5">
-        <v>0</v>
-      </c>
-      <c r="N34" s="5">
-        <v>0</v>
-      </c>
-      <c r="O34" s="5">
-        <v>0</v>
-      </c>
-      <c r="P34" s="22">
+      <c r="H34" s="19">
+        <v>0</v>
+      </c>
+      <c r="I34" s="19">
+        <v>0</v>
+      </c>
+      <c r="J34" s="19">
+        <v>0</v>
+      </c>
+      <c r="K34" s="19">
+        <v>0</v>
+      </c>
+      <c r="L34" s="19">
+        <v>0</v>
+      </c>
+      <c r="M34" s="19">
+        <v>0</v>
+      </c>
+      <c r="N34" s="19">
+        <v>0</v>
+      </c>
+      <c r="O34" s="19">
+        <v>0</v>
+      </c>
+      <c r="P34" s="21">
         <v>1</v>
       </c>
-      <c r="Q34" s="5">
-        <v>0</v>
-      </c>
-      <c r="R34" s="5">
-        <v>0</v>
-      </c>
-      <c r="S34" s="5">
-        <v>0</v>
-      </c>
-      <c r="T34" s="5">
-        <v>0</v>
+      <c r="Q34" s="19">
+        <v>0</v>
+      </c>
+      <c r="R34" s="19">
+        <v>0</v>
+      </c>
+      <c r="S34" s="19">
+        <v>0</v>
+      </c>
+      <c r="T34" s="19">
+        <v>0</v>
+      </c>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
elec by usage from RTE
</commit_message>
<xml_diff>
--- a/Concordances/IEA_sectors_pathways_concordance .xlsx
+++ b/Concordances/IEA_sectors_pathways_concordance .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cstbgroup-my.sharepoint.com/personal/marin_pellan_cstb_fr/Documents/Thèse stratégie carbone/Articles/Journal_papers/Carbon_budgets_Building_Environment/French_WLC_budgets/Concordances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="11_AD4D9D64A577C15A4A5418E8901D7D545ADEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{569E790A-B7F7-4800-8C7D-C7595CEFA9D5}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="11_AD4D9D64A577C15A4A5418E8901D7D545ADEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1175BE2F-49D9-420F-B9ED-3B1AB287B006}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -368,7 +368,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -715,7 +714,7 @@
     <col min="19" max="19" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23" style="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.109375" style="5"/>
-    <col min="22" max="16384" width="9.109375" style="28"/>
+    <col min="22" max="16384" width="9.109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -911,135 +910,135 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="19">
-        <v>0</v>
-      </c>
-      <c r="C4" s="19">
-        <v>0</v>
-      </c>
-      <c r="D4" s="19">
-        <v>0</v>
-      </c>
-      <c r="E4" s="19">
-        <v>0</v>
-      </c>
-      <c r="F4" s="19">
-        <v>0</v>
-      </c>
-      <c r="G4" s="20">
-        <v>0</v>
-      </c>
-      <c r="H4" s="19">
-        <v>0</v>
-      </c>
-      <c r="I4" s="19">
-        <v>0</v>
-      </c>
-      <c r="J4" s="19">
-        <v>0</v>
-      </c>
-      <c r="K4" s="19">
-        <v>0</v>
-      </c>
-      <c r="L4" s="19">
-        <v>0</v>
-      </c>
-      <c r="M4" s="19">
-        <v>0</v>
-      </c>
-      <c r="N4" s="19">
-        <v>0</v>
-      </c>
-      <c r="O4" s="21">
+      <c r="B4" s="18">
+        <v>0</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0</v>
+      </c>
+      <c r="K4" s="18">
+        <v>0</v>
+      </c>
+      <c r="L4" s="18">
+        <v>0</v>
+      </c>
+      <c r="M4" s="18">
+        <v>0</v>
+      </c>
+      <c r="N4" s="18">
+        <v>0</v>
+      </c>
+      <c r="O4" s="20">
         <v>1</v>
       </c>
-      <c r="P4" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="19">
-        <v>0</v>
-      </c>
-      <c r="R4" s="19">
-        <v>0</v>
-      </c>
-      <c r="S4" s="19">
-        <v>0</v>
-      </c>
-      <c r="T4" s="19">
-        <v>0</v>
-      </c>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19">
+      <c r="P4" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>0</v>
+      </c>
+      <c r="R4" s="18">
+        <v>0</v>
+      </c>
+      <c r="S4" s="18">
+        <v>0</v>
+      </c>
+      <c r="T4" s="18">
+        <v>0</v>
+      </c>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:23" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="17">
+      <c r="B5" s="18">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0</v>
+      </c>
+      <c r="F5" s="18">
+        <v>0</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
         <v>1</v>
       </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <v>0</v>
-      </c>
-      <c r="P5" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>0</v>
-      </c>
-      <c r="R5" s="5">
-        <v>0</v>
-      </c>
-      <c r="S5" s="5">
-        <v>0</v>
-      </c>
-      <c r="T5" s="5">
-        <v>0</v>
-      </c>
-      <c r="W5" s="5">
+      <c r="I5" s="18">
+        <v>0</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0</v>
+      </c>
+      <c r="L5" s="18">
+        <v>0</v>
+      </c>
+      <c r="M5" s="18">
+        <v>0</v>
+      </c>
+      <c r="N5" s="18">
+        <v>0</v>
+      </c>
+      <c r="O5" s="18">
+        <v>0</v>
+      </c>
+      <c r="P5" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>0</v>
+      </c>
+      <c r="R5" s="18">
+        <v>0</v>
+      </c>
+      <c r="S5" s="18">
+        <v>0</v>
+      </c>
+      <c r="T5" s="18">
+        <v>0</v>
+      </c>
+      <c r="W5" s="18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1373,69 +1372,69 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="19">
-        <v>0</v>
-      </c>
-      <c r="C11" s="19">
-        <v>0</v>
-      </c>
-      <c r="D11" s="19">
-        <v>0</v>
-      </c>
-      <c r="E11" s="19">
-        <v>0</v>
-      </c>
-      <c r="F11" s="21">
+      <c r="B11" s="18">
+        <v>0</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20">
         <v>1</v>
       </c>
-      <c r="G11" s="20">
-        <v>0</v>
-      </c>
-      <c r="H11" s="19">
-        <v>0</v>
-      </c>
-      <c r="I11" s="19">
-        <v>0</v>
-      </c>
-      <c r="J11" s="19">
-        <v>0</v>
-      </c>
-      <c r="K11" s="19">
-        <v>0</v>
-      </c>
-      <c r="L11" s="19">
-        <v>0</v>
-      </c>
-      <c r="M11" s="19">
-        <v>0</v>
-      </c>
-      <c r="N11" s="19">
-        <v>0</v>
-      </c>
-      <c r="O11" s="19">
-        <v>0</v>
-      </c>
-      <c r="P11" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="19">
-        <v>0</v>
-      </c>
-      <c r="R11" s="19">
-        <v>0</v>
-      </c>
-      <c r="S11" s="21">
+      <c r="G11" s="19">
+        <v>0</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18">
+        <v>0</v>
+      </c>
+      <c r="L11" s="18">
+        <v>0</v>
+      </c>
+      <c r="M11" s="18">
+        <v>0</v>
+      </c>
+      <c r="N11" s="18">
+        <v>0</v>
+      </c>
+      <c r="O11" s="18">
+        <v>0</v>
+      </c>
+      <c r="P11" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>0</v>
+      </c>
+      <c r="R11" s="18">
+        <v>0</v>
+      </c>
+      <c r="S11" s="20">
         <v>1</v>
       </c>
-      <c r="T11" s="19">
-        <v>0</v>
-      </c>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19">
+      <c r="T11" s="18">
+        <v>0</v>
+      </c>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1771,69 +1770,69 @@
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="26">
         <v>1</v>
       </c>
-      <c r="C17" s="19">
-        <v>0</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0</v>
-      </c>
-      <c r="E17" s="19">
+      <c r="C17" s="18">
+        <v>0</v>
+      </c>
+      <c r="D17" s="18">
+        <v>0</v>
+      </c>
+      <c r="E17" s="18">
         <v>1</v>
       </c>
-      <c r="F17" s="19">
-        <v>0</v>
-      </c>
-      <c r="G17" s="20">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
-        <v>0</v>
-      </c>
-      <c r="I17" s="19">
-        <v>0</v>
-      </c>
-      <c r="J17" s="19">
-        <v>0</v>
-      </c>
-      <c r="K17" s="19">
-        <v>0</v>
-      </c>
-      <c r="L17" s="19">
-        <v>0</v>
-      </c>
-      <c r="M17" s="19">
-        <v>0</v>
-      </c>
-      <c r="N17" s="19">
-        <v>0</v>
-      </c>
-      <c r="O17" s="19">
-        <v>0</v>
-      </c>
-      <c r="P17" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="19">
-        <v>0</v>
-      </c>
-      <c r="R17" s="19">
-        <v>0</v>
-      </c>
-      <c r="S17" s="19">
-        <v>0</v>
-      </c>
-      <c r="T17" s="19">
-        <v>0</v>
-      </c>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="19">
+      <c r="F17" s="18">
+        <v>0</v>
+      </c>
+      <c r="G17" s="19">
+        <v>0</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0</v>
+      </c>
+      <c r="I17" s="18">
+        <v>0</v>
+      </c>
+      <c r="J17" s="18">
+        <v>0</v>
+      </c>
+      <c r="K17" s="18">
+        <v>0</v>
+      </c>
+      <c r="L17" s="18">
+        <v>0</v>
+      </c>
+      <c r="M17" s="18">
+        <v>0</v>
+      </c>
+      <c r="N17" s="18">
+        <v>0</v>
+      </c>
+      <c r="O17" s="18">
+        <v>0</v>
+      </c>
+      <c r="P17" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>0</v>
+      </c>
+      <c r="R17" s="18">
+        <v>0</v>
+      </c>
+      <c r="S17" s="18">
+        <v>0</v>
+      </c>
+      <c r="T17" s="18">
+        <v>0</v>
+      </c>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2103,135 +2102,135 @@
       </c>
     </row>
     <row r="22" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="19">
-        <v>0</v>
-      </c>
-      <c r="C22" s="19">
-        <v>0</v>
-      </c>
-      <c r="D22" s="21">
+      <c r="B22" s="18">
+        <v>0</v>
+      </c>
+      <c r="C22" s="18">
+        <v>0</v>
+      </c>
+      <c r="D22" s="20">
         <v>1</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="19">
-        <v>0</v>
-      </c>
-      <c r="G22" s="23">
-        <v>0</v>
-      </c>
-      <c r="H22" s="19">
-        <v>0</v>
-      </c>
-      <c r="I22" s="19">
-        <v>0</v>
-      </c>
-      <c r="J22" s="21">
+      <c r="E22" s="20"/>
+      <c r="F22" s="18">
+        <v>0</v>
+      </c>
+      <c r="G22" s="22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="18">
+        <v>0</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0</v>
+      </c>
+      <c r="J22" s="20">
         <v>1</v>
       </c>
-      <c r="K22" s="21">
+      <c r="K22" s="20">
         <v>1</v>
       </c>
-      <c r="L22" s="21">
+      <c r="L22" s="20">
         <v>1</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M22" s="20">
         <v>1</v>
       </c>
-      <c r="N22" s="21">
+      <c r="N22" s="20">
         <v>1</v>
       </c>
-      <c r="O22" s="19">
-        <v>0</v>
-      </c>
-      <c r="P22" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="19">
-        <v>0</v>
-      </c>
-      <c r="R22" s="21">
+      <c r="O22" s="18">
+        <v>0</v>
+      </c>
+      <c r="P22" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>0</v>
+      </c>
+      <c r="R22" s="20">
         <v>1</v>
       </c>
-      <c r="S22" s="19">
-        <v>0</v>
-      </c>
-      <c r="T22" s="21">
+      <c r="S22" s="18">
+        <v>0</v>
+      </c>
+      <c r="T22" s="20">
         <v>1</v>
       </c>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-      <c r="W22" s="19">
+      <c r="U22" s="18"/>
+      <c r="V22" s="18"/>
+      <c r="W22" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="19">
-        <v>0</v>
-      </c>
-      <c r="C23" s="19">
-        <v>0</v>
-      </c>
-      <c r="D23" s="19">
-        <v>0</v>
-      </c>
-      <c r="E23" s="19">
-        <v>0</v>
-      </c>
-      <c r="F23" s="19">
-        <v>0</v>
-      </c>
-      <c r="G23" s="23">
-        <v>0</v>
-      </c>
-      <c r="H23" s="19">
-        <v>0</v>
-      </c>
-      <c r="I23" s="21">
+      <c r="B23" s="18">
+        <v>0</v>
+      </c>
+      <c r="C23" s="18">
+        <v>0</v>
+      </c>
+      <c r="D23" s="18">
+        <v>0</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0</v>
+      </c>
+      <c r="F23" s="18">
+        <v>0</v>
+      </c>
+      <c r="G23" s="22">
+        <v>0</v>
+      </c>
+      <c r="H23" s="18">
+        <v>0</v>
+      </c>
+      <c r="I23" s="20">
         <v>1</v>
       </c>
-      <c r="J23" s="19">
-        <v>0</v>
-      </c>
-      <c r="K23" s="19">
-        <v>0</v>
-      </c>
-      <c r="L23" s="19">
-        <v>0</v>
-      </c>
-      <c r="M23" s="19">
-        <v>0</v>
-      </c>
-      <c r="N23" s="19">
-        <v>0</v>
-      </c>
-      <c r="O23" s="19">
-        <v>0</v>
-      </c>
-      <c r="P23" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="19">
-        <v>0</v>
-      </c>
-      <c r="R23" s="19">
-        <v>0</v>
-      </c>
-      <c r="S23" s="19">
-        <v>0</v>
-      </c>
-      <c r="T23" s="19">
-        <v>0</v>
-      </c>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19">
+      <c r="J23" s="18">
+        <v>0</v>
+      </c>
+      <c r="K23" s="18">
+        <v>0</v>
+      </c>
+      <c r="L23" s="18">
+        <v>0</v>
+      </c>
+      <c r="M23" s="18">
+        <v>0</v>
+      </c>
+      <c r="N23" s="18">
+        <v>0</v>
+      </c>
+      <c r="O23" s="18">
+        <v>0</v>
+      </c>
+      <c r="P23" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="18">
+        <v>0</v>
+      </c>
+      <c r="R23" s="18">
+        <v>0</v>
+      </c>
+      <c r="S23" s="18">
+        <v>0</v>
+      </c>
+      <c r="T23" s="18">
+        <v>0</v>
+      </c>
+      <c r="U23" s="18"/>
+      <c r="V23" s="18"/>
+      <c r="W23" s="18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2303,202 +2302,202 @@
       </c>
     </row>
     <row r="25" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="19">
-        <v>0</v>
-      </c>
-      <c r="C25" s="21">
+      <c r="B25" s="18">
+        <v>0</v>
+      </c>
+      <c r="C25" s="20">
         <v>1</v>
       </c>
-      <c r="D25" s="19">
-        <v>0</v>
-      </c>
-      <c r="E25" s="19">
-        <v>0</v>
-      </c>
-      <c r="F25" s="19">
-        <v>0</v>
-      </c>
-      <c r="G25" s="23">
-        <v>0</v>
-      </c>
-      <c r="H25" s="19">
-        <v>0</v>
-      </c>
-      <c r="I25" s="19">
-        <v>0</v>
-      </c>
-      <c r="J25" s="19">
-        <v>0</v>
-      </c>
-      <c r="K25" s="19">
-        <v>0</v>
-      </c>
-      <c r="L25" s="19">
-        <v>0</v>
-      </c>
-      <c r="M25" s="19">
-        <v>0</v>
-      </c>
-      <c r="N25" s="19">
-        <v>0</v>
-      </c>
-      <c r="O25" s="19">
-        <v>0</v>
-      </c>
-      <c r="P25" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="19">
-        <v>0</v>
-      </c>
-      <c r="R25" s="19">
-        <v>0</v>
-      </c>
-      <c r="S25" s="19">
-        <v>0</v>
-      </c>
-      <c r="T25" s="19">
-        <v>0</v>
-      </c>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19">
+      <c r="D25" s="18">
+        <v>0</v>
+      </c>
+      <c r="E25" s="18">
+        <v>0</v>
+      </c>
+      <c r="F25" s="18">
+        <v>0</v>
+      </c>
+      <c r="G25" s="22">
+        <v>0</v>
+      </c>
+      <c r="H25" s="18">
+        <v>0</v>
+      </c>
+      <c r="I25" s="18">
+        <v>0</v>
+      </c>
+      <c r="J25" s="18">
+        <v>0</v>
+      </c>
+      <c r="K25" s="18">
+        <v>0</v>
+      </c>
+      <c r="L25" s="18">
+        <v>0</v>
+      </c>
+      <c r="M25" s="18">
+        <v>0</v>
+      </c>
+      <c r="N25" s="18">
+        <v>0</v>
+      </c>
+      <c r="O25" s="18">
+        <v>0</v>
+      </c>
+      <c r="P25" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="18">
+        <v>0</v>
+      </c>
+      <c r="R25" s="18">
+        <v>0</v>
+      </c>
+      <c r="S25" s="18">
+        <v>0</v>
+      </c>
+      <c r="T25" s="18">
+        <v>0</v>
+      </c>
+      <c r="U25" s="18"/>
+      <c r="V25" s="18"/>
+      <c r="W25" s="18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="28">
-        <v>0</v>
-      </c>
-      <c r="C26" s="28">
-        <v>0</v>
-      </c>
-      <c r="D26" s="28">
-        <v>0</v>
-      </c>
-      <c r="E26" s="28">
-        <v>0</v>
-      </c>
-      <c r="F26" s="28">
-        <v>0</v>
-      </c>
-      <c r="G26" s="30">
-        <v>0</v>
-      </c>
-      <c r="H26" s="28">
-        <v>0</v>
-      </c>
-      <c r="I26" s="28">
-        <v>0</v>
-      </c>
-      <c r="J26" s="28">
-        <v>0</v>
-      </c>
-      <c r="K26" s="28">
-        <v>0</v>
-      </c>
-      <c r="L26" s="28">
-        <v>0</v>
-      </c>
-      <c r="M26" s="28">
-        <v>0</v>
-      </c>
-      <c r="N26" s="28">
-        <v>0</v>
-      </c>
-      <c r="O26" s="28">
-        <v>0</v>
-      </c>
-      <c r="P26" s="28">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="31">
-        <v>0</v>
-      </c>
-      <c r="R26" s="28">
-        <v>0</v>
-      </c>
-      <c r="S26" s="28">
-        <v>0</v>
-      </c>
-      <c r="T26" s="28">
-        <v>0</v>
-      </c>
-      <c r="U26" s="28"/>
-      <c r="W26" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+      <c r="B26" s="27">
+        <v>0</v>
+      </c>
+      <c r="C26" s="27">
+        <v>0</v>
+      </c>
+      <c r="D26" s="27">
+        <v>0</v>
+      </c>
+      <c r="E26" s="27">
+        <v>0</v>
+      </c>
+      <c r="F26" s="27">
+        <v>0</v>
+      </c>
+      <c r="G26" s="29">
+        <v>0</v>
+      </c>
+      <c r="H26" s="27">
+        <v>0</v>
+      </c>
+      <c r="I26" s="27">
+        <v>0</v>
+      </c>
+      <c r="J26" s="27">
+        <v>0</v>
+      </c>
+      <c r="K26" s="27">
+        <v>0</v>
+      </c>
+      <c r="L26" s="27">
+        <v>0</v>
+      </c>
+      <c r="M26" s="27">
+        <v>0</v>
+      </c>
+      <c r="N26" s="27">
+        <v>0</v>
+      </c>
+      <c r="O26" s="27">
+        <v>0</v>
+      </c>
+      <c r="P26" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="30">
+        <v>0</v>
+      </c>
+      <c r="R26" s="27">
+        <v>0</v>
+      </c>
+      <c r="S26" s="27">
+        <v>0</v>
+      </c>
+      <c r="T26" s="27">
+        <v>0</v>
+      </c>
+      <c r="U26" s="27"/>
+      <c r="W26" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="19">
-        <v>0</v>
-      </c>
-      <c r="C27" s="19">
-        <v>0</v>
-      </c>
-      <c r="D27" s="19">
-        <v>0</v>
-      </c>
-      <c r="E27" s="19">
-        <v>0</v>
-      </c>
-      <c r="F27" s="19">
-        <v>0</v>
-      </c>
-      <c r="G27" s="19">
-        <v>0</v>
-      </c>
-      <c r="H27" s="19">
-        <v>0</v>
-      </c>
-      <c r="I27" s="19">
-        <v>0</v>
-      </c>
-      <c r="J27" s="19">
-        <v>0</v>
-      </c>
-      <c r="K27" s="19">
-        <v>0</v>
-      </c>
-      <c r="L27" s="19">
-        <v>0</v>
-      </c>
-      <c r="M27" s="19">
-        <v>0</v>
-      </c>
-      <c r="N27" s="19">
-        <v>0</v>
-      </c>
-      <c r="O27" s="19">
-        <v>0</v>
-      </c>
-      <c r="P27" s="19">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="21">
+      <c r="B27" s="18">
+        <v>0</v>
+      </c>
+      <c r="C27" s="18">
+        <v>0</v>
+      </c>
+      <c r="D27" s="18">
+        <v>0</v>
+      </c>
+      <c r="E27" s="18">
+        <v>0</v>
+      </c>
+      <c r="F27" s="18">
+        <v>0</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0</v>
+      </c>
+      <c r="H27" s="18">
+        <v>0</v>
+      </c>
+      <c r="I27" s="18">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18">
+        <v>0</v>
+      </c>
+      <c r="K27" s="18">
+        <v>0</v>
+      </c>
+      <c r="L27" s="18">
+        <v>0</v>
+      </c>
+      <c r="M27" s="18">
+        <v>0</v>
+      </c>
+      <c r="N27" s="18">
+        <v>0</v>
+      </c>
+      <c r="O27" s="18">
+        <v>0</v>
+      </c>
+      <c r="P27" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="20">
         <v>1</v>
       </c>
-      <c r="R27" s="19">
-        <v>0</v>
-      </c>
-      <c r="S27" s="19">
-        <v>0</v>
-      </c>
-      <c r="T27" s="19">
-        <v>0</v>
-      </c>
-      <c r="W27" s="19">
+      <c r="R27" s="18">
+        <v>0</v>
+      </c>
+      <c r="S27" s="18">
+        <v>0</v>
+      </c>
+      <c r="T27" s="18">
+        <v>0</v>
+      </c>
+      <c r="W27" s="18">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2900,69 +2899,69 @@
       </c>
     </row>
     <row r="34" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="19">
-        <v>0</v>
-      </c>
-      <c r="C34" s="19">
-        <v>0</v>
-      </c>
-      <c r="D34" s="19">
-        <v>0</v>
-      </c>
-      <c r="E34" s="19">
-        <v>0</v>
-      </c>
-      <c r="F34" s="19">
-        <v>0</v>
-      </c>
-      <c r="G34" s="21">
+      <c r="B34" s="18">
+        <v>0</v>
+      </c>
+      <c r="C34" s="18">
+        <v>0</v>
+      </c>
+      <c r="D34" s="18">
+        <v>0</v>
+      </c>
+      <c r="E34" s="18">
+        <v>0</v>
+      </c>
+      <c r="F34" s="18">
+        <v>0</v>
+      </c>
+      <c r="G34" s="20">
         <v>1</v>
       </c>
-      <c r="H34" s="19">
-        <v>0</v>
-      </c>
-      <c r="I34" s="19">
-        <v>0</v>
-      </c>
-      <c r="J34" s="19">
-        <v>0</v>
-      </c>
-      <c r="K34" s="19">
-        <v>0</v>
-      </c>
-      <c r="L34" s="19">
-        <v>0</v>
-      </c>
-      <c r="M34" s="19">
-        <v>0</v>
-      </c>
-      <c r="N34" s="19">
-        <v>0</v>
-      </c>
-      <c r="O34" s="19">
-        <v>0</v>
-      </c>
-      <c r="P34" s="21">
+      <c r="H34" s="18">
+        <v>0</v>
+      </c>
+      <c r="I34" s="18">
+        <v>0</v>
+      </c>
+      <c r="J34" s="18">
+        <v>0</v>
+      </c>
+      <c r="K34" s="18">
+        <v>0</v>
+      </c>
+      <c r="L34" s="18">
+        <v>0</v>
+      </c>
+      <c r="M34" s="18">
+        <v>0</v>
+      </c>
+      <c r="N34" s="18">
+        <v>0</v>
+      </c>
+      <c r="O34" s="18">
+        <v>0</v>
+      </c>
+      <c r="P34" s="20">
         <v>1</v>
       </c>
-      <c r="Q34" s="19">
-        <v>0</v>
-      </c>
-      <c r="R34" s="19">
-        <v>0</v>
-      </c>
-      <c r="S34" s="19">
-        <v>0</v>
-      </c>
-      <c r="T34" s="19">
-        <v>0</v>
-      </c>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19">
+      <c r="Q34" s="18">
+        <v>0</v>
+      </c>
+      <c r="R34" s="18">
+        <v>0</v>
+      </c>
+      <c r="S34" s="18">
+        <v>0</v>
+      </c>
+      <c r="T34" s="18">
+        <v>0</v>
+      </c>
+      <c r="U34" s="18"/>
+      <c r="V34" s="18"/>
+      <c r="W34" s="18">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>

</xml_diff>